<commit_message>
The cleaning of not localized text #1 and fix #30
</commit_message>
<xml_diff>
--- a/dev_info/gk_roadmap_ru.xlsx
+++ b/dev_info/gk_roadmap_ru.xlsx
@@ -1315,8 +1315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2086,5 +2086,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A18:A37" twoDigitTextYear="1"/>
+    <ignoredError sqref="A50 A63 A38 A2:A3" numberStoredAsText="1"/>
+    <ignoredError sqref="A4:A6" twoDigitTextYear="1" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Restored the execution of Lua scripts for Linux
</commit_message>
<xml_diff>
--- a/dev_info/gk_roadmap_ru.xlsx
+++ b/dev_info/gk_roadmap_ru.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="156">
   <si>
     <t>Добавить возможность задания модификатора лет в событиях.</t>
   </si>
@@ -222,9 +222,6 @@
   </si>
   <si>
     <t>Скрипты</t>
-  </si>
-  <si>
-    <t>Зависимость на lua.dll, dll-depend</t>
   </si>
   <si>
     <t>1.22</t>
@@ -492,7 +489,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -516,8 +513,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,12 +549,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -591,10 +589,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -615,25 +614,23 @@
     <xf numFmtId="2" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Процентный" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -961,7 +958,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -976,7 +973,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>9</v>
@@ -991,7 +988,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -1006,7 +1003,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -1021,7 +1018,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
@@ -1036,7 +1033,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>0</v>
@@ -1051,7 +1048,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>1</v>
@@ -1066,7 +1063,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -1081,7 +1078,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>10</v>
@@ -1096,7 +1093,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>11</v>
@@ -1111,7 +1108,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>3</v>
@@ -1126,7 +1123,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>6</v>
@@ -1141,7 +1138,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>14</v>
@@ -1156,7 +1153,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
@@ -1171,7 +1168,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>2</v>
@@ -1186,7 +1183,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>4</v>
@@ -1201,7 +1198,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>7</v>
@@ -1315,8 +1312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1559,7 +1556,7 @@
         <v>57</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C20" s="8">
         <v>1</v>
@@ -1571,11 +1568,11 @@
         <v>58</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C21" s="15"/>
+        <v>148</v>
+      </c>
+      <c r="C21" s="14"/>
       <c r="D21" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1583,11 +1580,11 @@
         <v>59</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C22" s="15"/>
+        <v>149</v>
+      </c>
+      <c r="C22" s="14"/>
       <c r="D22" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1597,9 +1594,9 @@
       <c r="B23" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="15"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1640,24 +1637,22 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="12">
-        <v>0</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="C27" s="8">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C28" s="8">
         <v>1</v>
@@ -1666,10 +1661,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C29" s="8">
         <v>1</v>
@@ -1678,10 +1673,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C30" s="8">
         <v>1</v>
@@ -1690,10 +1685,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C31" s="8">
         <v>1</v>
@@ -1702,10 +1697,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C32" s="8">
         <v>1</v>
@@ -1714,10 +1709,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C33" s="8">
         <v>1</v>
@@ -1726,10 +1721,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C34" s="8">
         <v>1</v>
@@ -1738,10 +1733,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C35" s="8">
         <v>1</v>
@@ -1750,10 +1745,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C36" s="8">
         <v>1</v>
@@ -1762,28 +1757,28 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B37" s="1"/>
-      <c r="C37" s="13"/>
+      <c r="C37" s="12"/>
       <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="C39" s="8">
         <v>1</v>
@@ -1792,10 +1787,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="C40" s="8">
         <v>1</v>
@@ -1804,10 +1799,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="C41" s="8">
         <v>1</v>
@@ -1816,10 +1811,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="C42" s="8">
         <v>1</v>
@@ -1828,10 +1823,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="C43" s="8">
         <v>1</v>
@@ -1840,10 +1835,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="C44" s="8">
         <v>1</v>
@@ -1852,10 +1847,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="C45" s="8">
         <v>1</v>
@@ -1864,10 +1859,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="C46" s="8">
         <v>1</v>
@@ -1876,24 +1871,24 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="C47" s="11">
         <v>0.75</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="C48" s="8">
         <v>1</v>
@@ -1902,42 +1897,42 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B49" s="1"/>
-      <c r="C49" s="13"/>
+      <c r="C49" s="12"/>
       <c r="D49" s="1"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>113</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>114</v>
       </c>
       <c r="C50" s="6"/>
       <c r="D50" s="5"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="C51" s="14">
-        <v>0.9</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="C52" s="8">
         <v>1</v>
@@ -1946,10 +1941,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="C53" s="8">
         <v>1</v>
@@ -1958,10 +1953,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="C54" s="8">
         <v>1</v>
@@ -1970,10 +1965,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="C55" s="8">
         <v>1</v>
@@ -1982,10 +1977,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="C56" s="8">
         <v>1</v>
@@ -1994,24 +1989,24 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="C57" s="11">
         <v>0.75</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="C58" s="8">
         <v>1</v>
@@ -2020,22 +2015,22 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" s="14"/>
+      <c r="D59" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C59" s="15"/>
-      <c r="D59" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="C60" s="8">
         <v>1</v>
@@ -2044,42 +2039,42 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" s="14"/>
+      <c r="D61" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="C61" s="15"/>
-      <c r="D61" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B62" s="1"/>
-      <c r="C62" s="13"/>
+      <c r="C62" s="12"/>
       <c r="D62" s="1"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>156</v>
-      </c>
       <c r="C63" s="8">
         <v>1</v>
       </c>
       <c r="D63" s="5"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="16"/>
+      <c r="A64" s="15"/>
       <c r="B64" s="2"/>
-      <c r="C64" s="17">
+      <c r="C64" s="16">
         <f>AVERAGE(C2:C63)</f>
-        <v>0.96862745098039216</v>
+        <v>0.98823529411764699</v>
       </c>
       <c r="D64" s="2"/>
     </row>

</xml_diff>

<commit_message>
Minor planning, cleaning and refactoring
</commit_message>
<xml_diff>
--- a/dev_info/gk_roadmap_ru.xlsx
+++ b/dev_info/gk_roadmap_ru.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="162">
   <si>
     <t>Добавить возможность задания модификатора лет в событиях.</t>
   </si>
@@ -489,6 +489,18 @@
   </si>
   <si>
     <t>Диалог настроек: слайд-список + страницы без табов</t>
+  </si>
+  <si>
+    <t>Обработка отчеств и фамилий в зависимости от культуры</t>
+  </si>
+  <si>
+    <t>Интерфейс с меньшим количеством диалогов</t>
+  </si>
+  <si>
+    <t>Встроенный чат с доской объявлений.</t>
+  </si>
+  <si>
+    <t>Backup-файлы при сохранении</t>
   </si>
 </sst>
 </file>
@@ -965,7 +977,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,16 +1000,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="19">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="D2" s="18">
+        <v>0</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1005,16 +1017,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="19">
-        <v>2</v>
+        <v>161</v>
+      </c>
+      <c r="D3" s="18">
+        <v>0</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1022,16 +1034,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="19">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="D4" s="17">
+        <v>1</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1039,16 +1051,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="18">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="D5" s="17">
+        <v>1</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1056,16 +1068,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="20">
-        <v>3</v>
+        <v>158</v>
+      </c>
+      <c r="D6" s="17">
+        <v>1</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1073,16 +1085,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="20">
-        <v>3</v>
+        <v>159</v>
+      </c>
+      <c r="D7" s="17">
+        <v>1</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1090,16 +1102,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="20">
-        <v>3</v>
+      <c r="D8" s="19">
+        <v>2</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1107,16 +1119,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="17">
-        <v>1</v>
+      <c r="D9" s="19">
+        <v>2</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1124,16 +1136,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="20">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="D10" s="19">
+        <v>2</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1141,16 +1153,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="20">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="D11" s="19">
+        <v>2</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1158,13 +1170,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>141</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D12" s="19">
         <v>2</v>
@@ -1175,13 +1187,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="D13" s="19">
         <v>2</v>
@@ -1192,13 +1204,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D14" s="19">
         <v>2</v>
@@ -1209,13 +1221,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D15" s="20">
         <v>3</v>
@@ -1226,16 +1238,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D16" s="19">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="D16" s="20">
+        <v>3</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1243,13 +1255,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17" s="20">
         <v>3</v>
@@ -1260,16 +1272,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="19">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="D18" s="20">
+        <v>3</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1277,13 +1289,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>157</v>
+        <v>10</v>
       </c>
       <c r="D19" s="20">
         <v>3</v>
@@ -1293,43 +1305,77 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="A20" s="2">
+        <v>14</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="20">
+        <v>3</v>
+      </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="A21" s="2">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="20">
+        <v>3</v>
+      </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="A22" s="2">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" s="20">
+        <v>3</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" s="20">
+        <v>3</v>
+      </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1374,8 +1420,8 @@
       <c r="G28" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D19">
-    <sortCondition ref="A2:A19"/>
+  <sortState ref="A2:D23">
+    <sortCondition ref="D2:D23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Small cleaning and fixing
</commit_message>
<xml_diff>
--- a/dev_info/gk_roadmap_ru.xlsx
+++ b/dev_info/gk_roadmap_ru.xlsx
@@ -623,7 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -667,6 +667,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -977,7 +981,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1102,13 +1106,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>143</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" s="19">
         <v>2</v>
@@ -1119,13 +1123,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D9" s="19">
         <v>2</v>
@@ -1136,13 +1140,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D10" s="19">
         <v>2</v>
@@ -1153,13 +1157,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>141</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D11" s="19">
         <v>2</v>
@@ -1170,13 +1174,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>155</v>
       </c>
       <c r="D12" s="19">
         <v>2</v>
@@ -1187,13 +1191,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>140</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>155</v>
+        <v>6</v>
       </c>
       <c r="D13" s="19">
         <v>2</v>
@@ -1204,16 +1208,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="19">
-        <v>2</v>
+        <v>15</v>
+      </c>
+      <c r="D14" s="20">
+        <v>3</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1221,13 +1225,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D15" s="20">
         <v>3</v>
@@ -1238,13 +1242,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="20">
         <v>3</v>
@@ -1255,13 +1259,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D17" s="20">
         <v>3</v>
@@ -1272,13 +1276,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>144</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D18" s="20">
         <v>3</v>
@@ -1289,13 +1293,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D19" s="20">
         <v>3</v>
@@ -1306,13 +1310,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D20" s="20">
         <v>3</v>
@@ -1323,13 +1327,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>3</v>
+        <v>157</v>
       </c>
       <c r="D21" s="20">
         <v>3</v>
@@ -1340,13 +1344,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>156</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D22" s="20">
         <v>3</v>
@@ -1356,21 +1360,19 @@
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>21</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D23" s="20">
-        <v>3</v>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="A23" s="21">
+        <v>1</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="22"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
@@ -1420,7 +1422,7 @@
       <c r="G28" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D23">
+  <sortState ref="A2:G23">
     <sortCondition ref="D2:D23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
A preliminary implementation of the autosave and lock it when the database is modifying
</commit_message>
<xml_diff>
--- a/dev_info/gk_roadmap_ru.xlsx
+++ b/dev_info/gk_roadmap_ru.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="171">
   <si>
     <t>Добавить возможность задания модификатора лет в событиях.</t>
   </si>
@@ -522,6 +522,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>GEDCOM API</t>
+  </si>
+  <si>
+    <t>Tree and base context locks</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1014,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1161,13 +1167,11 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>142</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>166</v>
@@ -1181,19 +1185,17 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>144</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>170</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="E9" s="20">
-        <v>3</v>
+      <c r="E9" s="19">
+        <v>2</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1201,13 +1203,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>157</v>
+        <v>9</v>
       </c>
       <c r="D10" s="24" t="s">
         <v>166</v>
@@ -1221,19 +1223,19 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>2</v>
+        <v>157</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>167</v>
-      </c>
-      <c r="E11" s="19">
-        <v>2</v>
+        <v>166</v>
+      </c>
+      <c r="E11" s="20">
+        <v>3</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1241,13 +1243,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>141</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>167</v>
@@ -1261,13 +1263,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>155</v>
+        <v>13</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>167</v>
@@ -1281,13 +1283,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>140</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>6</v>
+        <v>155</v>
       </c>
       <c r="D14" s="24" t="s">
         <v>167</v>
@@ -1301,19 +1303,19 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D15" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="E15" s="20">
-        <v>3</v>
+      <c r="E15" s="19">
+        <v>2</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1321,13 +1323,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>167</v>
@@ -1341,13 +1343,13 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>167</v>
@@ -1361,13 +1363,13 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>167</v>
@@ -1381,13 +1383,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>167</v>
@@ -1401,13 +1403,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D20" s="24" t="s">
         <v>167</v>
@@ -1421,16 +1423,16 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>160</v>
+        <v>3</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E21" s="20">
         <v>3</v>
@@ -1440,30 +1442,34 @@
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="21">
-        <v>22</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="E22" s="20">
+        <v>3</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="22"/>
@@ -1472,29 +1478,41 @@
       <c r="H23" s="21"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="A24" s="21">
+        <v>22</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="A25" s="21">
+        <v>1</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="21"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1504,7 +1522,9 @@
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1514,7 +1534,9 @@
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1524,9 +1546,9 @@
       <c r="H28" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A2:H21">
-    <sortCondition descending="1" ref="D2:D21"/>
-    <sortCondition ref="E2:E21"/>
+  <sortState ref="A2:H25">
+    <sortCondition descending="1" ref="D2:D25"/>
+    <sortCondition ref="E2:E25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Improvement of tests and other small changes
</commit_message>
<xml_diff>
--- a/dev_info/gk_roadmap_ru.xlsx
+++ b/dev_info/gk_roadmap_ru.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="ROADMAP" sheetId="1" r:id="rId1"/>
@@ -770,7 +770,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -805,7 +805,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1017,18 +1017,18 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="84.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>16</v>
       </c>
@@ -1048,7 +1048,7 @@
       <c r="G1" s="23"/>
       <c r="H1" s="23"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>4</v>
       </c>
@@ -1068,7 +1068,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>8</v>
       </c>
@@ -1088,7 +1088,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>12</v>
       </c>
@@ -1108,15 +1108,15 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>166</v>
@@ -1128,35 +1128,33 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>159</v>
+        <v>8</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="E6" s="17">
-        <v>1</v>
+      <c r="E6" s="19">
+        <v>2</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>143</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>166</v>
@@ -1168,109 +1166,109 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>23</v>
-      </c>
-      <c r="B8" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="C8" s="1" t="s">
-        <v>169</v>
+        <v>9</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="E8" s="19">
-        <v>2</v>
+      <c r="E8" s="20">
+        <v>3</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>24</v>
-      </c>
-      <c r="B9" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>156</v>
+      </c>
       <c r="C9" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="E9" s="19">
-        <v>2</v>
+      <c r="E9" s="20">
+        <v>3</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="24" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="21">
+        <v>19</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="E10" s="20">
-        <v>3</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>18</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D11" s="24" t="s">
+      <c r="E10" s="22"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
+        <v>24</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="D11" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="E11" s="20">
-        <v>3</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="21">
-        <v>11</v>
-      </c>
-      <c r="B12" s="21" t="s">
+      <c r="E11" s="22"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="E12" s="19">
         <v>2</v>
       </c>
-      <c r="D12" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>155</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>167</v>
@@ -1282,15 +1280,15 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>140</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>155</v>
+        <v>6</v>
       </c>
       <c r="D14" s="24" t="s">
         <v>167</v>
@@ -1302,35 +1300,35 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D15" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="E15" s="19">
-        <v>2</v>
+      <c r="E15" s="20">
+        <v>3</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>167</v>
@@ -1342,15 +1340,15 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>167</v>
@@ -1362,15 +1360,15 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>167</v>
@@ -1382,15 +1380,15 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>167</v>
@@ -1402,15 +1400,15 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D20" s="24" t="s">
         <v>167</v>
@@ -1422,27 +1420,25 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>16</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="24" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="21">
+        <v>11</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="E21" s="20">
-        <v>3</v>
-      </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E21" s="22"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1462,7 +1458,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="21">
         <v>3</v>
       </c>
@@ -1478,7 +1474,7 @@
       <c r="G23" s="21"/>
       <c r="H23" s="21"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="21">
         <v>22</v>
       </c>
@@ -1494,7 +1490,7 @@
       <c r="G24" s="21"/>
       <c r="H24" s="21"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="21">
         <v>1</v>
       </c>
@@ -1510,7 +1506,7 @@
       <c r="G25" s="21"/>
       <c r="H25" s="21"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1522,7 +1518,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1534,7 +1530,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1564,14 +1560,14 @@
       <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="60.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="60.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -1585,7 +1581,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -1595,7 +1591,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
@@ -1607,7 +1603,7 @@
       </c>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
@@ -1619,7 +1615,7 @@
       </c>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>26</v>
       </c>
@@ -1631,7 +1627,7 @@
       </c>
       <c r="D5" s="10"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>28</v>
       </c>
@@ -1643,7 +1639,7 @@
       </c>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>30</v>
       </c>
@@ -1655,7 +1651,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>32</v>
       </c>
@@ -1667,7 +1663,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>34</v>
       </c>
@@ -1679,7 +1675,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>36</v>
       </c>
@@ -1691,7 +1687,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>38</v>
       </c>
@@ -1703,7 +1699,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>40</v>
       </c>
@@ -1715,7 +1711,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>42</v>
       </c>
@@ -1727,7 +1723,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>44</v>
       </c>
@@ -1739,7 +1735,7 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>46</v>
       </c>
@@ -1751,7 +1747,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>48</v>
       </c>
@@ -1763,7 +1759,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>50</v>
       </c>
@@ -1775,7 +1771,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>52</v>
       </c>
@@ -1787,7 +1783,7 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -1799,7 +1795,7 @@
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -1811,7 +1807,7 @@
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -1823,7 +1819,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -1835,7 +1831,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>60</v>
       </c>
@@ -1847,7 +1843,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>62</v>
       </c>
@@ -1859,7 +1855,7 @@
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>64</v>
       </c>
@@ -1871,7 +1867,7 @@
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>66</v>
       </c>
@@ -1883,7 +1879,7 @@
       </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>68</v>
       </c>
@@ -1895,7 +1891,7 @@
       </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>70</v>
       </c>
@@ -1907,7 +1903,7 @@
       </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>72</v>
       </c>
@@ -1919,7 +1915,7 @@
       </c>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>74</v>
       </c>
@@ -1931,7 +1927,7 @@
       </c>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>76</v>
       </c>
@@ -1943,7 +1939,7 @@
       </c>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>78</v>
       </c>
@@ -1955,7 +1951,7 @@
       </c>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>80</v>
       </c>
@@ -1967,7 +1963,7 @@
       </c>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>82</v>
       </c>
@@ -1979,7 +1975,7 @@
       </c>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>84</v>
       </c>
@@ -1991,7 +1987,7 @@
       </c>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>86</v>
       </c>
@@ -2003,7 +1999,7 @@
       </c>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>149</v>
       </c>
@@ -2011,7 +2007,7 @@
       <c r="C37" s="12"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>87</v>
       </c>
@@ -2021,7 +2017,7 @@
       <c r="C38" s="6"/>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>89</v>
       </c>
@@ -2033,7 +2029,7 @@
       </c>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>91</v>
       </c>
@@ -2045,7 +2041,7 @@
       </c>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>93</v>
       </c>
@@ -2057,7 +2053,7 @@
       </c>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>95</v>
       </c>
@@ -2069,7 +2065,7 @@
       </c>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>97</v>
       </c>
@@ -2081,7 +2077,7 @@
       </c>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>99</v>
       </c>
@@ -2093,7 +2089,7 @@
       </c>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>101</v>
       </c>
@@ -2105,7 +2101,7 @@
       </c>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>103</v>
       </c>
@@ -2117,7 +2113,7 @@
       </c>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>105</v>
       </c>
@@ -2131,7 +2127,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>108</v>
       </c>
@@ -2143,7 +2139,7 @@
       </c>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>110</v>
       </c>
@@ -2151,7 +2147,7 @@
       <c r="C49" s="12"/>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>111</v>
       </c>
@@ -2161,7 +2157,7 @@
       <c r="C50" s="6"/>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>113</v>
       </c>
@@ -2175,7 +2171,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>116</v>
       </c>
@@ -2187,7 +2183,7 @@
       </c>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>118</v>
       </c>
@@ -2199,7 +2195,7 @@
       </c>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>120</v>
       </c>
@@ -2211,7 +2207,7 @@
       </c>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>122</v>
       </c>
@@ -2223,7 +2219,7 @@
       </c>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>124</v>
       </c>
@@ -2235,7 +2231,7 @@
       </c>
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>126</v>
       </c>
@@ -2249,7 +2245,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>128</v>
       </c>
@@ -2261,7 +2257,7 @@
       </c>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>130</v>
       </c>
@@ -2273,7 +2269,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>133</v>
       </c>
@@ -2285,7 +2281,7 @@
       </c>
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>135</v>
       </c>
@@ -2297,7 +2293,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>138</v>
       </c>
@@ -2305,7 +2301,7 @@
       <c r="C62" s="12"/>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>153</v>
       </c>
@@ -2317,7 +2313,7 @@
       </c>
       <c r="D63" s="5"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="15"/>
       <c r="B64" s="2"/>
       <c r="C64" s="16">

</xml_diff>

<commit_message>
[EtoPort] Added sample plugin; minor improvements of tools, components and progression; updated roadmap
</commit_message>
<xml_diff>
--- a/dev_info/gk_roadmap_ru.xlsx
+++ b/dev_info/gk_roadmap_ru.xlsx
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="182">
   <si>
     <t>Добавить возможность задания модификатора лет в событиях.</t>
   </si>
@@ -285,9 +285,6 @@
     <t>1.13</t>
   </si>
   <si>
-    <t>Вывод и просмотр деревьев всех типов</t>
-  </si>
-  <si>
     <t>1.14</t>
   </si>
   <si>
@@ -477,12 +474,6 @@
     <t>EXPORTS</t>
   </si>
   <si>
-    <t>Генерация росписей (pdf)</t>
-  </si>
-  <si>
-    <t>Фамильная книга (pdf)</t>
-  </si>
-  <si>
     <t>1.32</t>
   </si>
   <si>
@@ -585,12 +576,6 @@
     <t>1.33</t>
   </si>
   <si>
-    <t>Генерация росписей (rtf)</t>
-  </si>
-  <si>
-    <t>Генерация росписей (html)</t>
-  </si>
-  <si>
     <t>Basic functionality</t>
   </si>
   <si>
@@ -696,15 +681,9 @@
     <t>Work of the lists of records (ListView)</t>
   </si>
   <si>
-    <t>Sending of logs by mail</t>
-  </si>
-  <si>
     <t>Running the second instance with the transfer of control to the first</t>
   </si>
   <si>
-    <t>Круг предков/потомков</t>
-  </si>
-  <si>
     <t>1.21.1</t>
   </si>
   <si>
@@ -724,6 +703,30 @@
   </si>
   <si>
     <t>Manage lists (SheetList)</t>
+  </si>
+  <si>
+    <t>FamilyBook (pdf)</t>
+  </si>
+  <si>
+    <t>Display and view all types of trees</t>
+  </si>
+  <si>
+    <t>Circle of ancestors / descendants</t>
+  </si>
+  <si>
+    <t>Pedigrees (html)</t>
+  </si>
+  <si>
+    <t>Pedigrees (rtf)</t>
+  </si>
+  <si>
+    <t>Pedigrees (pdf)</t>
+  </si>
+  <si>
+    <t>Sending of logs by default mail's client</t>
+  </si>
+  <si>
+    <t>Custom toolbars (in controls and panels)</t>
   </si>
 </sst>
 </file>
@@ -973,6 +976,9 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -983,9 +989,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1312,16 +1315,16 @@
         <v>16</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
@@ -1332,13 +1335,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E2" s="17">
         <v>0</v>
@@ -1352,13 +1355,13 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E3" s="16">
         <v>1</v>
@@ -1372,13 +1375,13 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E4" s="16">
         <v>1</v>
@@ -1392,13 +1395,13 @@
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="D5" s="23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E5" s="16">
         <v>1</v>
@@ -1412,13 +1415,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E6" s="18">
         <v>2</v>
@@ -1433,10 +1436,10 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E7" s="18">
         <v>2</v>
@@ -1450,13 +1453,13 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E8" s="19">
         <v>3</v>
@@ -1470,13 +1473,13 @@
         <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E9" s="19">
         <v>3</v>
@@ -1490,13 +1493,13 @@
         <v>19</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="20"/>
@@ -1509,10 +1512,10 @@
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="20"/>
@@ -1524,13 +1527,13 @@
         <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E12" s="18">
         <v>2</v>
@@ -1544,13 +1547,13 @@
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E13" s="18">
         <v>2</v>
@@ -1564,13 +1567,13 @@
         <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E14" s="18">
         <v>2</v>
@@ -1584,13 +1587,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E15" s="19">
         <v>3</v>
@@ -1604,13 +1607,13 @@
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E16" s="19">
         <v>3</v>
@@ -1624,13 +1627,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E17" s="19">
         <v>3</v>
@@ -1644,13 +1647,13 @@
         <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E18" s="19">
         <v>3</v>
@@ -1664,13 +1667,13 @@
         <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E19" s="19">
         <v>3</v>
@@ -1684,13 +1687,13 @@
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E20" s="19">
         <v>3</v>
@@ -1704,13 +1707,13 @@
         <v>11</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E21" s="21"/>
       <c r="F21" s="20"/>
@@ -1722,13 +1725,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E22" s="19">
         <v>3</v>
@@ -1742,7 +1745,7 @@
         <v>3</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>4</v>
@@ -1758,10 +1761,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="21"/>
@@ -1774,7 +1777,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>7</v>
@@ -1833,10 +1836,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1847,41 +1850,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32" t="s">
-        <v>124</v>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
       <c r="C2" s="22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="F2" s="32"/>
+        <v>118</v>
+      </c>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1893,7 +1896,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C4" s="7">
         <v>1</v>
@@ -1911,7 +1914,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
@@ -1929,7 +1932,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
@@ -1947,13 +1950,13 @@
         <v>21</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
       </c>
-      <c r="D7" s="25">
-        <v>0</v>
+      <c r="D7" s="7">
+        <v>1</v>
       </c>
       <c r="E7" s="25">
         <v>0</v>
@@ -1965,7 +1968,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C8" s="7">
         <v>1</v>
@@ -1983,7 +1986,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C9" s="7">
         <v>1</v>
@@ -2001,7 +2004,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C10" s="7">
         <v>1</v>
@@ -2019,7 +2022,7 @@
         <v>25</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C11" s="7">
         <v>1</v>
@@ -2037,7 +2040,7 @@
         <v>26</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C12" s="7">
         <v>1</v>
@@ -2055,7 +2058,7 @@
         <v>27</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C13" s="7">
         <v>1</v>
@@ -2073,7 +2076,7 @@
         <v>28</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C14" s="7">
         <v>1</v>
@@ -2091,7 +2094,7 @@
         <v>29</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C15" s="7">
         <v>1</v>
@@ -2109,7 +2112,7 @@
         <v>30</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C16" s="7">
         <v>1</v>
@@ -2124,10 +2127,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C17" s="7">
         <v>1</v>
@@ -2145,7 +2148,7 @@
         <v>31</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C18" s="7">
         <v>1</v>
@@ -2163,115 +2166,115 @@
         <v>32</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C19" s="7">
         <v>1</v>
       </c>
-      <c r="D19" s="36">
-        <v>0</v>
-      </c>
-      <c r="E19" s="36">
+      <c r="D19" s="32">
+        <v>0</v>
+      </c>
+      <c r="E19" s="32">
         <v>0</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="C20" s="7">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1</v>
+      </c>
+      <c r="E20" s="7">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="7">
-        <v>1</v>
-      </c>
-      <c r="D20" s="25">
-        <v>0</v>
-      </c>
-      <c r="E20" s="25">
-        <v>0</v>
-      </c>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="B21" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="C21" s="7">
+        <v>1</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="E21" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C21" s="7">
-        <v>1</v>
-      </c>
-      <c r="D21" s="25">
-        <v>0</v>
-      </c>
-      <c r="E21" s="25">
-        <v>0</v>
-      </c>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="B22" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" s="7">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7">
+        <v>1</v>
+      </c>
+      <c r="E22" s="7">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C22" s="7">
-        <v>1</v>
-      </c>
-      <c r="D22" s="7">
-        <v>1</v>
-      </c>
-      <c r="E22" s="7">
-        <v>1</v>
-      </c>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="B23" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="C23" s="7">
+        <v>1</v>
+      </c>
+      <c r="D23" s="7">
+        <v>1</v>
+      </c>
+      <c r="E23" s="25">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C23" s="7">
-        <v>1</v>
-      </c>
-      <c r="D23" s="7">
-        <v>1</v>
-      </c>
-      <c r="E23" s="25">
-        <v>0</v>
-      </c>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="B24" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="C24" s="7">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7">
+        <v>1</v>
+      </c>
+      <c r="E24" s="7">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" s="7">
-        <v>1</v>
-      </c>
-      <c r="D24" s="7">
-        <v>1</v>
-      </c>
-      <c r="E24" s="7">
-        <v>1</v>
-      </c>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>99</v>
+      <c r="B25" s="26" t="s">
+        <v>174</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="25">
@@ -2284,10 +2287,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="25">
@@ -2300,10 +2303,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C27" s="7">
         <v>1</v>
@@ -2318,15 +2321,15 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C28" s="7">
         <v>1</v>
       </c>
-      <c r="D28" s="36">
+      <c r="D28" s="32">
         <v>0</v>
       </c>
       <c r="E28" s="7">
@@ -2336,10 +2339,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C29" s="7">
         <v>1</v>
@@ -2354,10 +2357,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C30" s="7">
         <v>1</v>
@@ -2372,10 +2375,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C31" s="7">
         <v>1</v>
@@ -2383,17 +2386,17 @@
       <c r="D31" s="7">
         <v>1</v>
       </c>
-      <c r="E31" s="36">
+      <c r="E31" s="32">
         <v>0</v>
       </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C32" s="7">
         <v>1</v>
@@ -2408,16 +2411,16 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C33" s="7">
         <v>1</v>
       </c>
-      <c r="D33" s="25">
-        <v>0</v>
+      <c r="D33" s="7">
+        <v>1</v>
       </c>
       <c r="E33" s="7">
         <v>1</v>
@@ -2426,24 +2429,24 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>129</v>
-      </c>
-      <c r="C34" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="D34" s="34"/>
-      <c r="E34" s="35"/>
+        <v>126</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="D34" s="35"/>
+      <c r="E34" s="36"/>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C35" s="7">
         <v>1</v>
@@ -2451,22 +2454,22 @@
       <c r="D35" s="7">
         <v>1</v>
       </c>
-      <c r="E35" s="25">
-        <v>0</v>
+      <c r="E35" s="7">
+        <v>1</v>
       </c>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C36" s="7">
         <v>1</v>
       </c>
-      <c r="D36" s="36">
+      <c r="D36" s="32">
         <v>0</v>
       </c>
       <c r="E36" s="7">
@@ -2476,10 +2479,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C37" s="7">
         <v>1</v>
@@ -2494,15 +2497,15 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C38" s="7">
         <v>1</v>
       </c>
-      <c r="D38" s="36">
+      <c r="D38" s="32">
         <v>0</v>
       </c>
       <c r="E38" s="10">
@@ -2512,28 +2515,28 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C39" s="7">
         <v>1</v>
       </c>
-      <c r="D39" s="36">
-        <v>0</v>
-      </c>
-      <c r="E39" s="36">
+      <c r="D39" s="32">
+        <v>0</v>
+      </c>
+      <c r="E39" s="32">
         <v>0</v>
       </c>
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C40" s="7">
         <v>1</v>
@@ -2548,10 +2551,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C41" s="7">
         <v>1</v>
@@ -2566,68 +2569,66 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="B42" s="26"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
+        <v>157</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="C42" s="7">
+        <v>1</v>
+      </c>
+      <c r="D42" s="32">
+        <v>0</v>
+      </c>
+      <c r="E42" s="7">
+        <v>1</v>
+      </c>
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="27"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="B43" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="4"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B44" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C44" s="7">
-        <v>1</v>
-      </c>
-      <c r="D44" s="25">
-        <v>0</v>
-      </c>
-      <c r="E44" s="7">
-        <v>1</v>
-      </c>
-      <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>56</v>
+      <c r="B45" s="26" t="s">
+        <v>128</v>
       </c>
       <c r="C45" s="7">
         <v>1</v>
       </c>
-      <c r="D45" s="25">
-        <v>0</v>
-      </c>
-      <c r="E45" s="25">
-        <v>0</v>
+      <c r="D45" s="7">
+        <v>1</v>
+      </c>
+      <c r="E45" s="7">
+        <v>1</v>
       </c>
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C46" s="7">
         <v>1</v>
@@ -2642,10 +2643,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C47" s="7">
         <v>1</v>
@@ -2660,10 +2661,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C48" s="7">
         <v>1</v>
@@ -2678,10 +2679,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C49" s="7">
         <v>1</v>
@@ -2696,10 +2697,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C50" s="7">
         <v>1</v>
@@ -2714,10 +2715,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C51" s="7">
         <v>1</v>
@@ -2732,13 +2733,13 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C52" s="10">
-        <v>0.75</v>
+        <v>67</v>
+      </c>
+      <c r="C52" s="7">
+        <v>1</v>
       </c>
       <c r="D52" s="25">
         <v>0</v>
@@ -2746,19 +2747,17 @@
       <c r="E52" s="25">
         <v>0</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="F52" s="1"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C53" s="7">
-        <v>1</v>
+        <v>69</v>
+      </c>
+      <c r="C53" s="10">
+        <v>0.75</v>
       </c>
       <c r="D53" s="25">
         <v>0</v>
@@ -2766,59 +2765,59 @@
       <c r="E53" s="25">
         <v>0</v>
       </c>
-      <c r="F53" s="1"/>
+      <c r="F53" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C54" s="7">
+        <v>1</v>
+      </c>
+      <c r="D54" s="25">
+        <v>0</v>
+      </c>
+      <c r="E54" s="25">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="B54" s="1"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="B55" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="4"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="B56" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="C56" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="D56" s="25">
-        <v>0</v>
-      </c>
-      <c r="E56" s="25">
-        <v>0</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="B56" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="4"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="27" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="C57" s="7">
-        <v>1</v>
+        <v>143</v>
+      </c>
+      <c r="C57" s="12">
+        <v>0.9</v>
       </c>
       <c r="D57" s="25">
         <v>0</v>
@@ -2826,14 +2825,16 @@
       <c r="E57" s="25">
         <v>0</v>
       </c>
-      <c r="F57" s="1"/>
+      <c r="F57" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C58" s="7">
         <v>1</v>
@@ -2848,10 +2849,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C59" s="7">
         <v>1</v>
@@ -2866,10 +2867,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C60" s="7">
         <v>1</v>
@@ -2884,10 +2885,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C61" s="7">
         <v>1</v>
@@ -2902,13 +2903,13 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="C62" s="10">
-        <v>0.75</v>
+        <v>148</v>
+      </c>
+      <c r="C62" s="7">
+        <v>1</v>
       </c>
       <c r="D62" s="25">
         <v>0</v>
@@ -2916,19 +2917,17 @@
       <c r="E62" s="25">
         <v>0</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>101</v>
-      </c>
+      <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="C63" s="7">
-        <v>1</v>
+        <v>149</v>
+      </c>
+      <c r="C63" s="10">
+        <v>0.75</v>
       </c>
       <c r="D63" s="25">
         <v>0</v>
@@ -2936,104 +2935,126 @@
       <c r="E63" s="25">
         <v>0</v>
       </c>
-      <c r="F63" s="1"/>
+      <c r="F63" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="C64" s="13"/>
+        <v>150</v>
+      </c>
+      <c r="C64" s="7">
+        <v>1</v>
+      </c>
       <c r="D64" s="25">
         <v>0</v>
       </c>
       <c r="E64" s="25">
         <v>0</v>
       </c>
-      <c r="F64" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="F64" s="1"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="27" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="C65" s="7">
-        <v>1</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="C65" s="13"/>
       <c r="D65" s="25">
         <v>0</v>
       </c>
       <c r="E65" s="25">
         <v>0</v>
       </c>
-      <c r="F65" s="1"/>
+      <c r="F65" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B66" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="C66" s="7">
+        <v>1</v>
+      </c>
+      <c r="D66" s="25">
+        <v>0</v>
+      </c>
+      <c r="E66" s="25">
+        <v>0</v>
+      </c>
+      <c r="F66" s="1"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B67" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="C67" s="13"/>
+      <c r="D67" s="25">
+        <v>0</v>
+      </c>
+      <c r="E67" s="25">
+        <v>0</v>
+      </c>
+      <c r="F67" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B66" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="C66" s="13"/>
-      <c r="D66" s="25">
-        <v>0</v>
-      </c>
-      <c r="E66" s="25">
-        <v>0</v>
-      </c>
-      <c r="F66" s="1" t="s">
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B67" s="1"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="31"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="1"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C68" s="7">
-        <v>1</v>
-      </c>
-      <c r="D68" s="25">
-        <v>0</v>
-      </c>
-      <c r="E68" s="7"/>
-      <c r="F68" s="4"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="31"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="1"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="15">
-        <f>AVERAGE(C3:C68)</f>
-        <v>0.98909090909090902</v>
-      </c>
-      <c r="D69" s="15">
-        <f>AVERAGE(D3:D68)</f>
-        <v>0.37542372881355929</v>
-      </c>
-      <c r="E69" s="15">
-        <f>AVERAGE(E3:E68)</f>
-        <v>0.42931034482758618</v>
-      </c>
-      <c r="F69" s="2"/>
+      <c r="A69" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C69" s="7">
+        <v>1</v>
+      </c>
+      <c r="D69" s="25">
+        <v>0</v>
+      </c>
+      <c r="E69" s="25">
+        <v>0</v>
+      </c>
+      <c r="F69" s="4"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="14"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="15">
+        <f>AVERAGE(C3:C69)</f>
+        <v>0.98928571428571421</v>
+      </c>
+      <c r="D70" s="15">
+        <f>AVERAGE(D3:D69)</f>
+        <v>0.44916666666666666</v>
+      </c>
+      <c r="E70" s="15">
+        <f>AVERAGE(E3:E69)</f>
+        <v>0.47333333333333333</v>
+      </c>
+      <c r="F70" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3047,7 +3068,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="A29:A42 A20:A27 A17" twoDigitTextYear="1"/>
-    <ignoredError sqref="A55 A68 A43 A3:A4" numberStoredAsText="1"/>
+    <ignoredError sqref="A56 A69 A44 A3:A4" numberStoredAsText="1"/>
     <ignoredError sqref="A5:A7" twoDigitTextYear="1" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>

</xml_diff>